<commit_message>
REQ: create a job in Hudson using Hudson REST API
</commit_message>
<xml_diff>
--- a/ali-config-from-yehud.xlsx
+++ b/ali-config-from-yehud.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="24675" windowHeight="12180" tabRatio="954"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="24675" windowHeight="12180" tabRatio="954" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Release-backlog-item#1" sheetId="19" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="852">
   <si>
     <t>alex</t>
   </si>
@@ -2534,9 +2534,6 @@
     <t>First Build Time</t>
   </si>
   <si>
-    <t>Build Folder</t>
-  </si>
-  <si>
     <t>13/12/2012 10:00</t>
   </si>
   <si>
@@ -2588,9 +2585,6 @@
     <t>First SVN Revision</t>
   </si>
   <si>
-    <t>c:\zz\BuildFolder</t>
-  </si>
-  <si>
     <t>defects</t>
   </si>
   <si>
@@ -2618,9 +2612,6 @@
     <t>Should be defecs/requirements generated?</t>
   </si>
   <si>
-    <t>Hudson build folder</t>
-  </si>
-  <si>
     <t>The time of the very first generated build</t>
   </si>
   <si>
@@ -2661,6 +2652,33 @@
   </si>
   <si>
     <t>which revision it starts with</t>
+  </si>
+  <si>
+    <t>Hudson URL</t>
+  </si>
+  <si>
+    <t>Job Name</t>
+  </si>
+  <si>
+    <t>BookStore2</t>
+  </si>
+  <si>
+    <t>Hudson Job Folder</t>
+  </si>
+  <si>
+    <t>Hudson folder with all the jobs</t>
+  </si>
+  <si>
+    <t>c:\Users\panuska\.hudson\jobs\</t>
+  </si>
+  <si>
+    <t>Build template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c:\zz\ali-generator\build-template </t>
+  </si>
+  <si>
+    <t>Where to take files to copy</t>
   </si>
 </sst>
 </file>
@@ -2777,7 +2795,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -2801,6 +2819,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3107,7 +3127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -12287,9 +12307,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D48"/>
+  <dimension ref="B1:D51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -12301,7 +12321,7 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -12312,7 +12332,7 @@
         <v>797</v>
       </c>
       <c r="D3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -12323,7 +12343,7 @@
         <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -12338,17 +12358,13 @@
       <c r="B6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>435</v>
-      </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="7">
-        <v>782297327</v>
-      </c>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -12358,12 +12374,12 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>799</v>
@@ -12374,10 +12390,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="D10" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -12388,7 +12404,7 @@
         <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -12396,287 +12412,314 @@
         <v>798</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D12" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>803</v>
+      <c r="B13" s="19" t="s">
+        <v>843</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>821</v>
-      </c>
-      <c r="D13" t="s">
-        <v>831</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>802</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="D14" t="s">
-        <v>832</v>
+      <c r="B14" s="19" t="s">
+        <v>844</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>845</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>800</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>801</v>
+        <v>846</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>848</v>
       </c>
       <c r="D15" t="s">
-        <v>833</v>
+        <v>847</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>820</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>801</v>
+        <v>849</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>850</v>
       </c>
       <c r="D16" t="s">
-        <v>835</v>
+        <v>851</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>813</v>
+        <v>803</v>
       </c>
       <c r="D17" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>838</v>
+        <v>800</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>839</v>
+        <v>801</v>
       </c>
       <c r="D18" t="s">
-        <v>837</v>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D19" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>100</v>
+        <v>824</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D20" t="s">
+        <v>833</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>105</v>
+        <v>835</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D21" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0</v>
+        <v>99</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>23</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" s="7">
-        <v>923608927</v>
+        <v>99</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>23</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="C32" s="7">
+        <v>923608927</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="7">
-        <v>0</v>
+        <v>99</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>23</v>
+        <v>101</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>169</v>
+        <v>110</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="7">
-        <v>0</v>
+        <v>99</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>435</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="7">
-        <v>782297327</v>
+        <v>99</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="7">
+        <v>782297327</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C33" r:id="rId1"/>
-    <hyperlink ref="C34" r:id="rId2"/>
+    <hyperlink ref="C36" r:id="rId1"/>
+    <hyperlink ref="C37" r:id="rId2"/>
     <hyperlink ref="C10" r:id="rId3"/>
-    <hyperlink ref="C39" r:id="rId4"/>
-    <hyperlink ref="C40" r:id="rId5"/>
-    <hyperlink ref="C46" r:id="rId6"/>
-    <hyperlink ref="C6" r:id="rId7"/>
+    <hyperlink ref="C42" r:id="rId4"/>
+    <hyperlink ref="C43" r:id="rId5"/>
+    <hyperlink ref="C49" r:id="rId6"/>
+    <hyperlink ref="C13" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
@@ -13171,46 +13214,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>809</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>810</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -13218,22 +13261,22 @@
         <v>86400000</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>813</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>811</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>814</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>812</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>813</v>
       </c>
       <c r="F2" s="18">
         <v>0</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H2">
         <v>30000</v>
@@ -13265,11 +13308,11 @@
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="I3">
         <v>7</v>
@@ -13302,7 +13345,7 @@
       </c>
       <c r="F4" s="18"/>
       <c r="G4" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H4">
         <v>5000000</v>
@@ -13498,7 +13541,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I12">
         <v>19</v>
@@ -13541,7 +13584,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="I14">
         <v>14</v>
@@ -13574,7 +13617,7 @@
       </c>
       <c r="F15" s="18"/>
       <c r="G15" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H15">
         <v>7000000</v>
@@ -13717,7 +13760,7 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I23">
         <v>5</v>
@@ -13752,7 +13795,7 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I25">
         <v>33</v>
@@ -13978,7 +14021,7 @@
         <v>86400000</v>
       </c>
       <c r="G38" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I38">
         <v>66</v>
@@ -13993,7 +14036,7 @@
         <v>86400000</v>
       </c>
       <c r="G39" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I39">
         <v>2</v>
@@ -14274,7 +14317,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>